<commit_message>
standardaddition in wägeprotokoll - new constants used if no standards in wägeprotokoll - standards used automatically if in wägeprotokoll
</commit_message>
<xml_diff>
--- a/data/Inga_2018-11-09_WM_20181109-114911/Results.xlsx
+++ b/data/Inga_2018-11-09_WM_20181109-114911/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="143">
   <si>
     <t>Lab. #</t>
   </si>
@@ -30,15 +30,15 @@
     <t>Mess. Dat.</t>
   </si>
   <si>
-    <t>Tiefe (cm)</t>
-  </si>
-  <si>
     <t>Einwaage (g)</t>
   </si>
   <si>
     <t>TriSp13 (g)</t>
   </si>
   <si>
+    <t>Tiefe</t>
+  </si>
+  <si>
     <t>Ratio 233/236</t>
   </si>
   <si>
@@ -330,9 +330,6 @@
     <t>Bezeichnung</t>
   </si>
   <si>
-    <t>Tiefe</t>
-  </si>
-  <si>
     <t>d234U (initial)</t>
   </si>
   <si>
@@ -405,7 +402,7 @@
     <t>Taylor 1. Ord.</t>
   </si>
   <si>
-    <t>(cm)</t>
+    <t>cm</t>
   </si>
   <si>
     <t>(a BP)</t>
@@ -929,9 +926,9 @@
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
@@ -1082,10 +1079,10 @@
       <c r="D3" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="E3" s="4">
+        <v>1.0953</v>
+      </c>
       <c r="F3" s="4">
-        <v>1.0953</v>
-      </c>
-      <c r="G3" s="4">
         <v>10.34617</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -1159,10 +1156,10 @@
       <c r="D4" t="s">
         <v>34</v>
       </c>
+      <c r="E4">
+        <v>0.011411</v>
+      </c>
       <c r="F4">
-        <v>0.011411</v>
-      </c>
-      <c r="G4">
         <v>0.009849</v>
       </c>
       <c r="H4" t="s">
@@ -1233,10 +1230,10 @@
       <c r="D5" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="E5" s="4">
+        <v>1.0953</v>
+      </c>
       <c r="F5" s="4">
-        <v>1.0953</v>
-      </c>
-      <c r="G5" s="4">
         <v>10.34617</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -1310,10 +1307,10 @@
       <c r="D6" t="s">
         <v>34</v>
       </c>
+      <c r="E6">
+        <v>0.010943</v>
+      </c>
       <c r="F6">
-        <v>0.010943</v>
-      </c>
-      <c r="G6">
         <v>0.009334</v>
       </c>
       <c r="H6" t="s">
@@ -1384,10 +1381,10 @@
       <c r="D7" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="E7" s="4">
+        <v>1.0953</v>
+      </c>
       <c r="F7" s="4">
-        <v>1.0953</v>
-      </c>
-      <c r="G7" s="4">
         <v>10.34617</v>
       </c>
       <c r="H7" s="4" t="s">
@@ -1461,10 +1458,10 @@
       <c r="D8" t="s">
         <v>34</v>
       </c>
+      <c r="E8">
+        <v>0.006735</v>
+      </c>
       <c r="F8">
-        <v>0.006735</v>
-      </c>
-      <c r="G8">
         <v>0.009993</v>
       </c>
       <c r="H8" t="s">
@@ -1535,10 +1532,10 @@
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="E9" s="4">
+        <v>1.0953</v>
+      </c>
       <c r="F9" s="4">
-        <v>1.0953</v>
-      </c>
-      <c r="G9" s="4">
         <v>10.34617</v>
       </c>
       <c r="H9" s="4" t="s">
@@ -1612,10 +1609,10 @@
       <c r="D10" t="s">
         <v>34</v>
       </c>
+      <c r="E10">
+        <v>0.0124</v>
+      </c>
       <c r="F10">
-        <v>0.0124</v>
-      </c>
-      <c r="G10">
         <v>0.00962</v>
       </c>
       <c r="H10" t="s">
@@ -1686,10 +1683,10 @@
       <c r="D11" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="E11" s="4">
+        <v>1.0953</v>
+      </c>
       <c r="F11" s="4">
-        <v>1.0953</v>
-      </c>
-      <c r="G11" s="4">
         <v>10.34617</v>
       </c>
       <c r="H11" s="4" t="s">
@@ -1763,10 +1760,10 @@
       <c r="D12" t="s">
         <v>34</v>
       </c>
+      <c r="E12">
+        <v>0.0125</v>
+      </c>
       <c r="F12">
-        <v>0.0125</v>
-      </c>
-      <c r="G12">
         <v>0.009428000000000001</v>
       </c>
       <c r="H12" t="s">
@@ -1837,10 +1834,10 @@
       <c r="D13" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="E13" s="4">
+        <v>1.0953</v>
+      </c>
       <c r="F13" s="4">
-        <v>1.0953</v>
-      </c>
-      <c r="G13" s="4">
         <v>10.34617</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -1914,10 +1911,10 @@
       <c r="D14" t="s">
         <v>34</v>
       </c>
+      <c r="E14">
+        <v>0.01497</v>
+      </c>
       <c r="F14">
-        <v>0.01497</v>
-      </c>
-      <c r="G14">
         <v>0.010175</v>
       </c>
       <c r="H14" t="s">
@@ -1988,10 +1985,10 @@
       <c r="D15" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="E15" s="4">
+        <v>1.0953</v>
+      </c>
       <c r="F15" s="4">
-        <v>1.0953</v>
-      </c>
-      <c r="G15" s="4">
         <v>10.34617</v>
       </c>
       <c r="H15" s="4" t="s">
@@ -2065,10 +2062,10 @@
       <c r="D16" t="s">
         <v>34</v>
       </c>
+      <c r="E16">
+        <v>0.012018</v>
+      </c>
       <c r="F16">
-        <v>0.012018</v>
-      </c>
-      <c r="G16">
         <v>0.009748</v>
       </c>
       <c r="H16" t="s">
@@ -2139,10 +2136,10 @@
       <c r="D17" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="E17" s="4">
+        <v>1.0953</v>
+      </c>
       <c r="F17" s="4">
-        <v>1.0953</v>
-      </c>
-      <c r="G17" s="4">
         <v>10.34617</v>
       </c>
       <c r="H17" s="4" t="s">
@@ -2288,61 +2285,61 @@
         <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>57</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>59</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>64</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>69</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>71</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>73</v>
@@ -2351,13 +2348,13 @@
         <v>74</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>78</v>
@@ -2366,46 +2363,46 @@
         <v>79</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>84</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>86</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AL1" s="1" t="s">
         <v>88</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>90</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>92</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>94</v>
@@ -2414,46 +2411,46 @@
         <v>95</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>97</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AW1" s="1" t="s">
         <v>99</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BA1" s="1" t="s">
         <v>103</v>
       </c>
       <c r="BB1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BC1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BC1" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="BD1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BE1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BF1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:59" s="3" customFormat="1">
@@ -2461,163 +2458,163 @@
         <v>52</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>50</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN2" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="AL2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP2" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="AO2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="AQ2" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AR2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AU2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AY2" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="AZ2" s="3" t="s">
         <v>51</v>
       </c>
       <c r="BB2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="BE2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="BC2" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="BD2" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="BE2" s="3" t="s">
+      <c r="BF2" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="BF2" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="BG2" s="3" t="s">
         <v>51</v>
@@ -2649,16 +2646,16 @@
         <v>0</v>
       </c>
       <c r="J3" s="4">
-        <v>748.1857733049716</v>
+        <v>748.1857733049717</v>
       </c>
       <c r="K3" s="4">
-        <v>3.297010990930299</v>
+        <v>3.2970109909303</v>
       </c>
       <c r="L3" s="4">
-        <v>10.34710815653514</v>
+        <v>10.34710815653515</v>
       </c>
       <c r="M3" s="4">
-        <v>0.04559633520662432</v>
+        <v>0.04559633520662433</v>
       </c>
       <c r="N3" s="4">
         <v>0</v>
@@ -2670,10 +2667,10 @@
         <v>0.001537435798429116</v>
       </c>
       <c r="Q3" s="4">
-        <v>10.34710815653514</v>
+        <v>10.34710815653515</v>
       </c>
       <c r="R3" s="4">
-        <v>0.04559633520662432</v>
+        <v>0.04559633520662433</v>
       </c>
       <c r="S3" s="4">
         <v>0.9979534204436099</v>
@@ -2691,16 +2688,16 @@
         <v>0</v>
       </c>
       <c r="X3" s="4">
-        <v>0.8905816135662882</v>
+        <v>0.8905816135662884</v>
       </c>
       <c r="Y3" s="4">
-        <v>0.003562470684003865</v>
+        <v>0.003562470684003866</v>
       </c>
       <c r="Z3" s="4">
         <v>0.000217459649863845</v>
       </c>
       <c r="AA3" s="4">
-        <v>8.69873817057004E-07</v>
+        <v>8.698738170570043E-07</v>
       </c>
       <c r="AB3" s="4">
         <v>0</v>
@@ -2712,7 +2709,7 @@
         <v>224.4377544158947</v>
       </c>
       <c r="AE3" s="4">
-        <v>0.8354738423200543</v>
+        <v>0.8354738423200544</v>
       </c>
       <c r="AF3" s="4">
         <v>10.2320259459459</v>
@@ -2721,10 +2718,10 @@
         <v>0.03808891268773317</v>
       </c>
       <c r="AH3" s="4">
-        <v>47052.52653700281</v>
+        <v>47052.5265370028</v>
       </c>
       <c r="AI3" s="4">
-        <v>257.1085613729377</v>
+        <v>257.1085613729376</v>
       </c>
       <c r="AJ3" s="4">
         <v>-2.046579556390093</v>
@@ -2733,31 +2730,31 @@
         <v>1.297592116384946</v>
       </c>
       <c r="AL3" s="4">
-        <v>0.9998560822461793</v>
+        <v>0.9998560822461795</v>
       </c>
       <c r="AM3" s="4">
         <v>0.003723670601000376</v>
       </c>
       <c r="AN3" s="4">
-        <v>0.9998560822461793</v>
+        <v>0.9998560822461795</v>
       </c>
       <c r="AO3" s="4">
         <v>0.003723670601000376</v>
       </c>
       <c r="AP3" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AQ3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AS3" s="4">
         <v>2.124978520462398E-05</v>
       </c>
       <c r="AT3" s="4">
-        <v>8.503595166371856E-08</v>
+        <v>8.503595166371861E-08</v>
       </c>
       <c r="AU3" s="4">
         <v>0.75</v>
@@ -2766,31 +2763,31 @@
         <v>0.375</v>
       </c>
       <c r="AW3" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AX3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AY3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AZ3" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BD3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE3" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BF3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BG3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:59">
@@ -2912,19 +2909,19 @@
         <v>0.007549738173726313</v>
       </c>
       <c r="AN4">
-        <v>0.9738301850808498</v>
+        <v>0.9738301850808496</v>
       </c>
       <c r="AO4">
-        <v>0.007540389817617558</v>
+        <v>0.007540389817617557</v>
       </c>
       <c r="AP4">
         <v>397.3046</v>
       </c>
       <c r="AQ4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AS4">
         <v>1.231864737557985E-07</v>
@@ -2942,13 +2939,13 @@
         <v>378.6177</v>
       </c>
       <c r="AX4">
-        <v>27.776555387</v>
+        <v>27.7695114754</v>
       </c>
       <c r="AY4">
-        <v>26.94013232986835</v>
+        <v>26.94013232986834</v>
       </c>
       <c r="AZ4">
-        <v>7.336306619315472</v>
+        <v>7.33444619081464</v>
       </c>
       <c r="BA4" t="s">
         <v>25</v>
@@ -2957,7 +2954,7 @@
         <v>11.15943581643624</v>
       </c>
       <c r="BD4">
-        <v>4.371332342713034</v>
+        <v>4.371287823590726</v>
       </c>
       <c r="BE4">
         <v>378559.7</v>
@@ -2966,7 +2963,7 @@
         <v>13470.06616493417</v>
       </c>
       <c r="BG4">
-        <v>3557.695840668351</v>
+        <v>3557.69584066835</v>
       </c>
     </row>
     <row r="5" spans="1:59" s="4" customFormat="1">
@@ -3037,16 +3034,16 @@
         <v>0</v>
       </c>
       <c r="X5" s="4">
-        <v>0.8885586414037057</v>
+        <v>0.8885586414037059</v>
       </c>
       <c r="Y5" s="4">
-        <v>0.003944462981395974</v>
+        <v>0.003944462981395975</v>
       </c>
       <c r="Z5" s="4">
         <v>0.0002169656863556631</v>
       </c>
       <c r="AA5" s="4">
-        <v>9.631475945257893E-07</v>
+        <v>9.631475945257896E-07</v>
       </c>
       <c r="AB5" s="4">
         <v>0</v>
@@ -3058,16 +3055,16 @@
         <v>225.0609455359863</v>
       </c>
       <c r="AE5" s="4">
-        <v>0.5196890915829907</v>
+        <v>0.5196890915829908</v>
       </c>
       <c r="AF5" s="4">
         <v>10.26043697566172</v>
       </c>
       <c r="AG5" s="4">
-        <v>0.02369241432993786</v>
+        <v>0.02369241432993787</v>
       </c>
       <c r="AH5" s="4">
-        <v>47290.59764244102</v>
+        <v>47290.59764244103</v>
       </c>
       <c r="AI5" s="4">
         <v>236.6335313630173</v>
@@ -3079,31 +3076,31 @@
         <v>1.114055567528818</v>
       </c>
       <c r="AL5" s="4">
-        <v>1.002623459617004</v>
+        <v>1.002623459617005</v>
       </c>
       <c r="AM5" s="4">
-        <v>0.002316701521823447</v>
+        <v>0.002316701521823448</v>
       </c>
       <c r="AN5" s="4">
-        <v>1.002623459617004</v>
+        <v>1.002623459617005</v>
       </c>
       <c r="AO5" s="4">
-        <v>0.002316701521823447</v>
+        <v>0.002316701521823448</v>
       </c>
       <c r="AP5" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AQ5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AS5" s="4">
         <v>2.120132773955892E-05</v>
       </c>
       <c r="AT5" s="4">
-        <v>9.413324231000063E-08</v>
+        <v>9.413324231000064E-08</v>
       </c>
       <c r="AU5" s="4">
         <v>0.75</v>
@@ -3112,31 +3109,31 @@
         <v>0.375</v>
       </c>
       <c r="AW5" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AX5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AY5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AZ5" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BD5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE5" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BF5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BG5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:59">
@@ -3171,28 +3168,28 @@
         <v>189.4517208163983</v>
       </c>
       <c r="K6">
-        <v>4.399843257982285</v>
+        <v>4.399843257982286</v>
       </c>
       <c r="L6">
-        <v>2.620041058880085</v>
+        <v>2.620041058880086</v>
       </c>
       <c r="M6">
-        <v>0.06084806165324896</v>
+        <v>0.06084806165324897</v>
       </c>
       <c r="N6">
         <v>0.005</v>
       </c>
       <c r="O6">
-        <v>3.441329043288853</v>
+        <v>3.441329043288854</v>
       </c>
       <c r="P6">
-        <v>0.0008901550723946611</v>
+        <v>0.0008901550723946612</v>
       </c>
       <c r="Q6">
-        <v>2.620041058880085</v>
+        <v>2.620041058880086</v>
       </c>
       <c r="R6">
-        <v>0.06084806165324896</v>
+        <v>0.06084806165324897</v>
       </c>
       <c r="S6">
         <v>1.001440140168575</v>
@@ -3216,10 +3213,10 @@
         <v>0.01043551771987159</v>
       </c>
       <c r="Z6">
-        <v>0.000585279046127846</v>
+        <v>0.0005852790461278461</v>
       </c>
       <c r="AA6">
-        <v>2.548114619640433E-06</v>
+        <v>2.548114619640434E-06</v>
       </c>
       <c r="AB6">
         <v>0.05</v>
@@ -3228,7 +3225,7 @@
         <v>0.85</v>
       </c>
       <c r="AD6">
-        <v>55.97238355680559</v>
+        <v>55.9723835568056</v>
       </c>
       <c r="AE6">
         <v>0.2461979722211669</v>
@@ -3255,22 +3252,22 @@
         <v>0.9937853020262534</v>
       </c>
       <c r="AM6">
-        <v>0.004378777677250769</v>
+        <v>0.004378777677250768</v>
       </c>
       <c r="AN6">
-        <v>0.9924465873509145</v>
+        <v>0.9924465873509143</v>
       </c>
       <c r="AO6">
-        <v>0.004372879085347034</v>
+        <v>0.004372879085347033</v>
       </c>
       <c r="AP6">
         <v>524.2474</v>
       </c>
       <c r="AQ6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AS6">
         <v>0.0002279376286621842</v>
@@ -3288,13 +3285,13 @@
         <v>478.1797</v>
       </c>
       <c r="AX6">
-        <v>45.5096899786</v>
+        <v>43.7967841768</v>
       </c>
       <c r="AY6">
-        <v>42.37518575336064</v>
+        <v>42.37518575336063</v>
       </c>
       <c r="AZ6">
-        <v>9.517277705138884</v>
+        <v>9.159063878454063</v>
       </c>
       <c r="BA6" t="s">
         <v>26</v>
@@ -3303,7 +3300,7 @@
         <v>13.98358006908092</v>
       </c>
       <c r="BD6">
-        <v>6.652995257658999</v>
+        <v>6.635013597763908</v>
       </c>
       <c r="BE6">
         <v>478121.7</v>
@@ -3312,7 +3309,7 @@
         <v>21187.59287668032</v>
       </c>
       <c r="BG6">
-        <v>4430.885057789011</v>
+        <v>4430.88505778901</v>
       </c>
     </row>
     <row r="7" spans="1:59" s="4" customFormat="1">
@@ -3341,7 +3338,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="4">
-        <v>753.5170186994569</v>
+        <v>753.517018699457</v>
       </c>
       <c r="K7" s="4">
         <v>3.068260342464981</v>
@@ -3404,19 +3401,19 @@
         <v>224.4687551531487</v>
       </c>
       <c r="AE7" s="4">
-        <v>0.734074506235452</v>
+        <v>0.7340745062354521</v>
       </c>
       <c r="AF7" s="4">
         <v>10.23343925694945</v>
       </c>
       <c r="AG7" s="4">
-        <v>0.03346615819431243</v>
+        <v>0.03346615819431244</v>
       </c>
       <c r="AH7" s="4">
-        <v>47126.27585529182</v>
+        <v>47126.27585529183</v>
       </c>
       <c r="AI7" s="4">
-        <v>264.2105267220917</v>
+        <v>264.2105267220918</v>
       </c>
       <c r="AJ7" s="4">
         <v>-0.760486846759223</v>
@@ -3428,7 +3425,7 @@
         <v>1.000074347383193</v>
       </c>
       <c r="AM7" s="4">
-        <v>0.003271868689528417</v>
+        <v>0.003271868689528416</v>
       </c>
       <c r="AN7" s="4">
         <v>1.000074347383193</v>
@@ -3437,19 +3434,19 @@
         <v>0.003271868689528417</v>
       </c>
       <c r="AP7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AQ7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AS7" s="4">
         <v>2.122116227588339E-05</v>
       </c>
       <c r="AT7" s="4">
-        <v>9.665833382527448E-08</v>
+        <v>9.665833382527447E-08</v>
       </c>
       <c r="AU7" s="4">
         <v>0.75</v>
@@ -3458,31 +3455,31 @@
         <v>0.375</v>
       </c>
       <c r="AW7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AX7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AY7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AZ7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BD7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BF7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BG7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:59">
@@ -3613,10 +3610,10 @@
         <v>404.9719</v>
       </c>
       <c r="AQ8">
-        <v>17.5533</v>
+        <v>17.6166</v>
       </c>
       <c r="AR8">
-        <v>4.334448883984296</v>
+        <v>4.350079598115326</v>
       </c>
       <c r="AS8">
         <v>-2.848827408654226E-06</v>
@@ -3634,13 +3631,13 @@
         <v>392.5668</v>
       </c>
       <c r="AX8">
-        <v>15.4711221581</v>
+        <v>15.4603560565</v>
       </c>
       <c r="AY8">
         <v>15.22732118483986</v>
       </c>
       <c r="AZ8">
-        <v>3.941016448181558</v>
+        <v>3.938273959107087</v>
       </c>
       <c r="BA8" t="s">
         <v>27</v>
@@ -3649,7 +3646,7 @@
         <v>1.561188494939421</v>
       </c>
       <c r="BD8">
-        <v>2.249848914858602</v>
+        <v>2.249847473994108</v>
       </c>
       <c r="BE8">
         <v>392508.8</v>
@@ -3687,16 +3684,16 @@
         <v>0</v>
       </c>
       <c r="J9" s="4">
-        <v>751.2003425705045</v>
+        <v>751.2003425705046</v>
       </c>
       <c r="K9" s="4">
-        <v>3.24737589967227</v>
+        <v>3.247375899672271</v>
       </c>
       <c r="L9" s="4">
         <v>10.38879843634099</v>
       </c>
       <c r="M9" s="4">
-        <v>0.04490990186890168</v>
+        <v>0.0449099018689017</v>
       </c>
       <c r="N9" s="4">
         <v>0</v>
@@ -3705,13 +3702,13 @@
         <v>13.71348592665002</v>
       </c>
       <c r="P9" s="4">
-        <v>0.0009364572733045003</v>
+        <v>0.0009364572733045004</v>
       </c>
       <c r="Q9" s="4">
         <v>10.38879843634099</v>
       </c>
       <c r="R9" s="4">
-        <v>0.04490990186890168</v>
+        <v>0.0449099018689017</v>
       </c>
       <c r="S9" s="4">
         <v>0.9981348389721758</v>
@@ -3750,19 +3747,19 @@
         <v>224.9781858373517</v>
       </c>
       <c r="AE9" s="4">
-        <v>0.701465843424813</v>
+        <v>0.7014658434248132</v>
       </c>
       <c r="AF9" s="4">
         <v>10.25666399465898</v>
       </c>
       <c r="AG9" s="4">
-        <v>0.03197954251857908</v>
+        <v>0.03197954251857909</v>
       </c>
       <c r="AH9" s="4">
-        <v>47324.15634140059</v>
+        <v>47324.1563414006</v>
       </c>
       <c r="AI9" s="4">
-        <v>264.5574770388683</v>
+        <v>264.5574770388684</v>
       </c>
       <c r="AJ9" s="4">
         <v>-1.865161027824191</v>
@@ -3780,22 +3777,22 @@
         <v>1.00239181729563</v>
       </c>
       <c r="AO9" s="4">
-        <v>0.00312613527074461</v>
+        <v>0.003126135270744611</v>
       </c>
       <c r="AP9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AQ9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AS9" s="4">
         <v>2.118139856660703E-05</v>
       </c>
       <c r="AT9" s="4">
-        <v>9.829386551335134E-08</v>
+        <v>9.829386551335133E-08</v>
       </c>
       <c r="AU9" s="4">
         <v>0.75</v>
@@ -3804,31 +3801,31 @@
         <v>0.375</v>
       </c>
       <c r="AW9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AX9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AY9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AZ9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BD9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BF9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BG9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:59">
@@ -3959,10 +3956,10 @@
         <v>397.7362</v>
       </c>
       <c r="AQ10">
-        <v>18.5615</v>
+        <v>18.7193</v>
       </c>
       <c r="AR10">
-        <v>4.666786679210994</v>
+        <v>4.706461217259078</v>
       </c>
       <c r="AS10">
         <v>2.420526768828991E-05</v>
@@ -3980,13 +3977,13 @@
         <v>382.7414</v>
       </c>
       <c r="AX10">
-        <v>15.6920625477</v>
+        <v>15.5550792921</v>
       </c>
       <c r="AY10">
         <v>15.44634142461242</v>
       </c>
       <c r="AZ10">
-        <v>4.0999125121296</v>
+        <v>4.064122483771026</v>
       </c>
       <c r="BA10" t="s">
         <v>28</v>
@@ -3995,7 +3992,7 @@
         <v>7.14257275472135</v>
       </c>
       <c r="BD10">
-        <v>1.872778622070147</v>
+        <v>1.872312863114833</v>
       </c>
       <c r="BE10">
         <v>382683.4</v>
@@ -4033,7 +4030,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="4">
-        <v>752.4124295904246</v>
+        <v>752.4124295904247</v>
       </c>
       <c r="K11" s="4">
         <v>3.627677316760044</v>
@@ -4042,7 +4039,7 @@
         <v>10.40556111205299</v>
       </c>
       <c r="M11" s="4">
-        <v>0.05016931742462463</v>
+        <v>0.05016931742462465</v>
       </c>
       <c r="N11" s="4">
         <v>0</v>
@@ -4057,7 +4054,7 @@
         <v>10.40556111205299</v>
       </c>
       <c r="R11" s="4">
-        <v>0.05016931742462463</v>
+        <v>0.05016931742462465</v>
       </c>
       <c r="S11" s="4">
         <v>0.9974728278637717</v>
@@ -4096,16 +4093,16 @@
         <v>224.3366590343894</v>
       </c>
       <c r="AE11" s="4">
-        <v>0.6444418154306463</v>
+        <v>0.6444418154306465</v>
       </c>
       <c r="AF11" s="4">
         <v>10.22741704861814</v>
       </c>
       <c r="AG11" s="4">
-        <v>0.0293798402737533</v>
+        <v>0.02937984027375331</v>
       </c>
       <c r="AH11" s="4">
-        <v>47242.52769689465</v>
+        <v>47242.52769689466</v>
       </c>
       <c r="AI11" s="4">
         <v>255.8755126776899</v>
@@ -4129,19 +4126,19 @@
         <v>0.002872367027651197</v>
       </c>
       <c r="AP11" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AQ11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AS11" s="4">
         <v>2.115829056715183E-05</v>
       </c>
       <c r="AT11" s="4">
-        <v>9.716385016702405E-08</v>
+        <v>9.716385016702404E-08</v>
       </c>
       <c r="AU11" s="4">
         <v>0.75</v>
@@ -4150,31 +4147,31 @@
         <v>0.375</v>
       </c>
       <c r="AW11" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AX11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AY11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AZ11" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BD11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE11" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BF11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BG11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:59">
@@ -4305,10 +4302,10 @@
         <v>420.0755</v>
       </c>
       <c r="AQ12">
-        <v>14.2781</v>
+        <v>14.0009</v>
       </c>
       <c r="AR12">
-        <v>3.398936619726693</v>
+        <v>3.332948481880043</v>
       </c>
       <c r="AS12">
         <v>0.0007162712758635274</v>
@@ -4326,13 +4323,13 @@
         <v>402.4051</v>
       </c>
       <c r="AX12">
-        <v>11.7405050166</v>
+        <v>11.7539290985</v>
       </c>
       <c r="AY12">
         <v>11.63508045267128</v>
       </c>
       <c r="AZ12">
-        <v>2.917583553637864</v>
+        <v>2.920919515806335</v>
       </c>
       <c r="BA12" t="s">
         <v>29</v>
@@ -4341,7 +4338,7 @@
         <v>8.180229292027676</v>
       </c>
       <c r="BD12">
-        <v>1.944806272615011</v>
+        <v>1.944849614308049</v>
       </c>
       <c r="BE12">
         <v>402347.1</v>
@@ -4397,7 +4394,7 @@
         <v>13.71439719886068</v>
       </c>
       <c r="P13" s="4">
-        <v>0.0009508093226944609</v>
+        <v>0.0009508093226944613</v>
       </c>
       <c r="Q13" s="4">
         <v>10.35955877906956</v>
@@ -4421,16 +4418,16 @@
         <v>0</v>
       </c>
       <c r="X13" s="4">
-        <v>0.8910975031795663</v>
+        <v>0.8910975031795665</v>
       </c>
       <c r="Y13" s="4">
-        <v>0.00289923583108927</v>
+        <v>0.002899235831089271</v>
       </c>
       <c r="Z13" s="4">
-        <v>0.000217585618301732</v>
+        <v>0.0002175856183017321</v>
       </c>
       <c r="AA13" s="4">
-        <v>7.079270435156577E-07</v>
+        <v>7.07927043515658E-07</v>
       </c>
       <c r="AB13" s="4">
         <v>0</v>
@@ -4439,7 +4436,7 @@
         <v>0.85</v>
       </c>
       <c r="AD13" s="4">
-        <v>224.723729225271</v>
+        <v>224.7237292252711</v>
       </c>
       <c r="AE13" s="4">
         <v>0.4849885220627204</v>
@@ -4451,7 +4448,7 @@
         <v>0.02211042947808194</v>
       </c>
       <c r="AH13" s="4">
-        <v>47085.20490078314</v>
+        <v>47085.20490078312</v>
       </c>
       <c r="AI13" s="4">
         <v>183.8329587987095</v>
@@ -4466,7 +4463,7 @@
         <v>1.001191554165284</v>
       </c>
       <c r="AM13" s="4">
-        <v>0.002161840651871306</v>
+        <v>0.002161840651871305</v>
       </c>
       <c r="AN13" s="4">
         <v>1.001191554165284</v>
@@ -4475,19 +4472,19 @@
         <v>0.002161840651871305</v>
       </c>
       <c r="AP13" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AQ13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AS13" s="4">
-        <v>2.126340017580834E-05</v>
+        <v>2.126340017580835E-05</v>
       </c>
       <c r="AT13" s="4">
-        <v>6.919737272673649E-08</v>
+        <v>6.919737272673651E-08</v>
       </c>
       <c r="AU13" s="4">
         <v>0.75</v>
@@ -4496,31 +4493,31 @@
         <v>0.375</v>
       </c>
       <c r="AW13" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AX13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AY13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AZ13" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BD13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE13" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BF13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BG13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:59">
@@ -4552,31 +4549,31 @@
         <v>0.3</v>
       </c>
       <c r="J14">
-        <v>450.5565472804185</v>
+        <v>450.5565472804184</v>
       </c>
       <c r="K14">
         <v>13.36014267472493</v>
       </c>
       <c r="L14">
-        <v>6.231015733902825</v>
+        <v>6.231015733902823</v>
       </c>
       <c r="M14">
-        <v>0.1847653967429442</v>
+        <v>0.1847653967429441</v>
       </c>
       <c r="N14">
         <v>0.005</v>
       </c>
       <c r="O14">
-        <v>7.181574108241955</v>
+        <v>7.181574108241954</v>
       </c>
       <c r="P14">
         <v>0.001784814193384784</v>
       </c>
       <c r="Q14">
-        <v>6.231015733902825</v>
+        <v>6.231015733902823</v>
       </c>
       <c r="R14">
-        <v>0.1847653967429442</v>
+        <v>0.1847653967429441</v>
       </c>
       <c r="S14">
         <v>0.9993542964288743</v>
@@ -4624,10 +4621,10 @@
         <v>0.01873924392169261</v>
       </c>
       <c r="AH14">
-        <v>60076.83976345309</v>
+        <v>60076.83976345308</v>
       </c>
       <c r="AI14">
-        <v>437.2998753640364</v>
+        <v>437.2998753640363</v>
       </c>
       <c r="AJ14">
         <v>1.712729973920579</v>
@@ -4636,25 +4633,25 @@
         <v>0.6823467466899904</v>
       </c>
       <c r="AL14">
-        <v>0.9801247180705144</v>
+        <v>0.9801247180705143</v>
       </c>
       <c r="AM14">
         <v>0.003505602211917841</v>
       </c>
       <c r="AN14">
-        <v>0.9800853014669939</v>
+        <v>0.9800853014669938</v>
       </c>
       <c r="AO14">
-        <v>0.00350546123094885</v>
+        <v>0.003505461230948849</v>
       </c>
       <c r="AP14">
         <v>432.7757</v>
       </c>
       <c r="AQ14">
-        <v>21.4986</v>
+        <v>21.9775</v>
       </c>
       <c r="AR14">
-        <v>4.967607931776207</v>
+        <v>5.07826571593553</v>
       </c>
       <c r="AS14">
         <v>1.631451857204313E-05</v>
@@ -4672,13 +4669,13 @@
         <v>415.719</v>
       </c>
       <c r="AX14">
-        <v>17.5169768967</v>
+        <v>17.8925037114</v>
       </c>
       <c r="AY14">
         <v>17.71232715398179</v>
       </c>
       <c r="AZ14">
-        <v>4.213657998960837</v>
+        <v>4.303989885331197</v>
       </c>
       <c r="BA14" t="s">
         <v>30</v>
@@ -4687,13 +4684,13 @@
         <v>5.545768381608759</v>
       </c>
       <c r="BD14">
-        <v>2.226412639016464</v>
+        <v>2.227146161265094</v>
       </c>
       <c r="BE14">
         <v>415661</v>
       </c>
       <c r="BF14">
-        <v>8856.163576990895</v>
+        <v>8856.163576990893</v>
       </c>
       <c r="BG14">
         <v>2130.324468448855</v>
@@ -4725,7 +4722,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="4">
-        <v>755.5153322885968</v>
+        <v>755.5153322885969</v>
       </c>
       <c r="K15" s="4">
         <v>3.400485079869327</v>
@@ -4740,10 +4737,10 @@
         <v>0</v>
       </c>
       <c r="O15" s="4">
-        <v>13.71319985415296</v>
+        <v>13.71319985415297</v>
       </c>
       <c r="P15" s="4">
-        <v>0.001149709602279575</v>
+        <v>0.001149709602279576</v>
       </c>
       <c r="Q15" s="4">
         <v>10.4484730076847</v>
@@ -4788,7 +4785,7 @@
         <v>224.1873052188604</v>
       </c>
       <c r="AE15" s="4">
-        <v>0.5298360637907557</v>
+        <v>0.5298360637907558</v>
       </c>
       <c r="AF15" s="4">
         <v>10.22060806890973</v>
@@ -4797,7 +4794,7 @@
         <v>0.02415501066615967</v>
       </c>
       <c r="AH15" s="4">
-        <v>46823.41662719673</v>
+        <v>46823.41662719674</v>
       </c>
       <c r="AI15" s="4">
         <v>226.7451110517479</v>
@@ -4809,31 +4806,31 @@
         <v>0.7914499647809169</v>
       </c>
       <c r="AL15" s="4">
-        <v>0.9988888808814648</v>
+        <v>0.9988888808814645</v>
       </c>
       <c r="AM15" s="4">
         <v>0.002362222359513692</v>
       </c>
       <c r="AN15" s="4">
-        <v>0.9988888808814648</v>
+        <v>0.9988888808814645</v>
       </c>
       <c r="AO15" s="4">
         <v>0.002362222359513692</v>
       </c>
       <c r="AP15" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AQ15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AS15" s="4">
         <v>2.133310537405922E-05</v>
       </c>
       <c r="AT15" s="4">
-        <v>9.018609275344029E-08</v>
+        <v>9.018609275344027E-08</v>
       </c>
       <c r="AU15" s="4">
         <v>0.75</v>
@@ -4842,31 +4839,31 @@
         <v>0.375</v>
       </c>
       <c r="AW15" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AX15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AY15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AZ15" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BD15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE15" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BF15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BG15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:59">
@@ -4898,10 +4895,10 @@
         <v>0.3</v>
       </c>
       <c r="J16">
-        <v>645.9444097648344</v>
+        <v>645.9444097648345</v>
       </c>
       <c r="K16">
-        <v>15.87283569557307</v>
+        <v>15.87283569557308</v>
       </c>
       <c r="L16">
         <v>8.933151243202859</v>
@@ -4940,16 +4937,16 @@
         <v>0.003</v>
       </c>
       <c r="X16">
-        <v>17.38770470481672</v>
+        <v>17.38770470481673</v>
       </c>
       <c r="Y16">
-        <v>0.03836494628929124</v>
+        <v>0.03836494628929125</v>
       </c>
       <c r="Z16">
-        <v>0.004245679586741138</v>
+        <v>0.00424567958674114</v>
       </c>
       <c r="AA16">
-        <v>9.367841936132127E-06</v>
+        <v>9.367841936132132E-06</v>
       </c>
       <c r="AB16">
         <v>0.05</v>
@@ -4970,10 +4967,10 @@
         <v>0.01967634679881496</v>
       </c>
       <c r="AH16">
-        <v>1972.290696569124</v>
+        <v>1972.290696569123</v>
       </c>
       <c r="AI16">
-        <v>6.357334532176222</v>
+        <v>6.357334532176221</v>
       </c>
       <c r="AJ16">
         <v>2.698465868033573</v>
@@ -4982,10 +4979,10 @@
         <v>0.5214580713338243</v>
       </c>
       <c r="AL16">
-        <v>0.9842607025012421</v>
+        <v>0.9842607025012419</v>
       </c>
       <c r="AM16">
-        <v>0.002321730393690571</v>
+        <v>0.00232173039369057</v>
       </c>
       <c r="AN16">
         <v>0.9845915147220022</v>
@@ -4997,10 +4994,10 @@
         <v>454.7034</v>
       </c>
       <c r="AQ16">
-        <v>17.4221</v>
+        <v>17.8032</v>
       </c>
       <c r="AR16">
-        <v>3.831530619740252</v>
+        <v>3.915343496441857</v>
       </c>
       <c r="AS16">
         <v>0.0004990444381314589</v>
@@ -5018,13 +5015,13 @@
         <v>432.406</v>
       </c>
       <c r="AX16">
-        <v>13.6931576438</v>
+        <v>13.9484281894</v>
       </c>
       <c r="AY16">
         <v>13.78076683895438</v>
       </c>
       <c r="AZ16">
-        <v>3.166736271883368</v>
+        <v>3.225771194062987</v>
       </c>
       <c r="BA16" t="s">
         <v>31</v>
@@ -5033,7 +5030,7 @@
         <v>9.159508245909548</v>
       </c>
       <c r="BD16">
-        <v>1.80515289220322</v>
+        <v>1.806462203862902</v>
       </c>
       <c r="BE16">
         <v>432348</v>
@@ -5089,7 +5086,7 @@
         <v>13.71319273712027</v>
       </c>
       <c r="P17" s="4">
-        <v>0.0008672834130371031</v>
+        <v>0.0008672834130371032</v>
       </c>
       <c r="Q17" s="4">
         <v>10.37808834239952</v>
@@ -5134,7 +5131,7 @@
         <v>224.5351238116349</v>
       </c>
       <c r="AE17" s="4">
-        <v>0.7610961640055035</v>
+        <v>0.7610961640055036</v>
       </c>
       <c r="AF17" s="4">
         <v>10.23646497709798</v>
@@ -5155,31 +5152,31 @@
         <v>1.018388305285391</v>
       </c>
       <c r="AL17" s="4">
-        <v>1.000439140504433</v>
+        <v>1.000439140504432</v>
       </c>
       <c r="AM17" s="4">
+        <v>0.003391731787599698</v>
+      </c>
+      <c r="AN17" s="4">
+        <v>1.000439140504432</v>
+      </c>
+      <c r="AO17" s="4">
         <v>0.003391731787599699</v>
       </c>
-      <c r="AN17" s="4">
-        <v>1.000439140504433</v>
-      </c>
-      <c r="AO17" s="4">
-        <v>0.0033917317875997</v>
-      </c>
       <c r="AP17" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AQ17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AR17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AS17" s="4">
-        <v>2.122696603498933E-05</v>
+        <v>2.122696603498932E-05</v>
       </c>
       <c r="AT17" s="4">
-        <v>9.517443744401181E-08</v>
+        <v>9.517443744401179E-08</v>
       </c>
       <c r="AU17" s="4">
         <v>0.75</v>
@@ -5188,31 +5185,31 @@
         <v>0.375</v>
       </c>
       <c r="AW17" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AX17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AY17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AZ17" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BC17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BD17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE17" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BF17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BG17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -5257,108 +5254,108 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>88</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>92</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>104</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="3" customFormat="1">
       <c r="C2" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="J2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="4" customFormat="1">
@@ -5372,22 +5369,22 @@
         <v>0.001537435798429116</v>
       </c>
       <c r="E3" s="4">
-        <v>0.8905816135662882</v>
+        <v>0.8905816135662884</v>
       </c>
       <c r="F3" s="4">
-        <v>0.003562470684003865</v>
+        <v>0.003562470684003866</v>
       </c>
       <c r="G3" s="4">
-        <v>0.9998560822461793</v>
+        <v>0.9998560822461795</v>
       </c>
       <c r="H3" s="4">
         <v>0.003723670601000376</v>
       </c>
       <c r="I3" s="4">
-        <v>47052.52653700281</v>
+        <v>47052.5265370028</v>
       </c>
       <c r="J3" s="4">
-        <v>257.1085613729377</v>
+        <v>257.1085613729376</v>
       </c>
       <c r="K3" s="4">
         <v>-2.046579556390093</v>
@@ -5396,16 +5393,16 @@
         <v>1.297592116384946</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q3" s="4">
         <v>-2.046579556390093</v>
@@ -5434,10 +5431,10 @@
         <v>0.0001659232090856783</v>
       </c>
       <c r="G4">
-        <v>0.9738301850808498</v>
+        <v>0.9738301850808496</v>
       </c>
       <c r="H4">
-        <v>0.007540389817617558</v>
+        <v>0.007540389817617557</v>
       </c>
       <c r="I4">
         <v>167.7946240138874</v>
@@ -5455,13 +5452,13 @@
         <v>397.3046</v>
       </c>
       <c r="N4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O4">
         <v>378.6177</v>
       </c>
       <c r="P4">
-        <v>27.776555387</v>
+        <v>27.7695114754</v>
       </c>
       <c r="Q4">
         <v>3.827447745538448</v>
@@ -5481,19 +5478,19 @@
         <v>0.001155277868178238</v>
       </c>
       <c r="E5" s="4">
-        <v>0.8885586414037057</v>
+        <v>0.8885586414037059</v>
       </c>
       <c r="F5" s="4">
-        <v>0.003944462981395974</v>
+        <v>0.003944462981395975</v>
       </c>
       <c r="G5" s="4">
-        <v>1.002623459617004</v>
+        <v>1.002623459617005</v>
       </c>
       <c r="H5" s="4">
-        <v>0.002316701521823447</v>
+        <v>0.002316701521823448</v>
       </c>
       <c r="I5" s="4">
-        <v>47290.59764244102</v>
+        <v>47290.59764244103</v>
       </c>
       <c r="J5" s="4">
         <v>236.6335313630173</v>
@@ -5505,16 +5502,16 @@
         <v>1.114055567528818</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q5" s="4">
         <v>-3.583007132901161</v>
@@ -5531,10 +5528,10 @@
         <v>26</v>
       </c>
       <c r="C6">
-        <v>3.441329043288853</v>
+        <v>3.441329043288854</v>
       </c>
       <c r="D6">
-        <v>0.0008901550723946611</v>
+        <v>0.0008901550723946612</v>
       </c>
       <c r="E6">
         <v>2.39694470957454</v>
@@ -5543,16 +5540,16 @@
         <v>0.01043551771987159</v>
       </c>
       <c r="G6">
-        <v>0.9924465873509145</v>
+        <v>0.9924465873509143</v>
       </c>
       <c r="H6">
-        <v>0.004372879085347034</v>
+        <v>0.004372879085347033</v>
       </c>
       <c r="I6">
-        <v>0.09235425811625793</v>
+        <v>0.09235425811625791</v>
       </c>
       <c r="J6">
-        <v>0.0005715663752333282</v>
+        <v>0.000571566375233328</v>
       </c>
       <c r="K6">
         <v>3.619748335957684</v>
@@ -5564,13 +5561,13 @@
         <v>524.2474</v>
       </c>
       <c r="N6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O6">
         <v>478.1797</v>
       </c>
       <c r="P6">
-        <v>45.5096899786</v>
+        <v>43.7967841768</v>
       </c>
       <c r="Q6">
         <v>3.619748335957684</v>
@@ -5602,7 +5599,7 @@
         <v>0.003271868689528417</v>
       </c>
       <c r="I7" s="4">
-        <v>47126.27585529182</v>
+        <v>47126.27585529183</v>
       </c>
       <c r="J7" s="4">
         <v>264.2105267220917</v>
@@ -5614,16 +5611,16 @@
         <v>0.9839394015774066</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q7" s="4">
         <v>-0.760486846759223</v>
@@ -5658,7 +5655,7 @@
         <v>0.003707114672799816</v>
       </c>
       <c r="I8">
-        <v>-7.242809029274999</v>
+        <v>-7.242809029274997</v>
       </c>
       <c r="J8">
         <v>-0.1110933018636352</v>
@@ -5673,13 +5670,13 @@
         <v>404.9719</v>
       </c>
       <c r="N8">
-        <v>17.5533</v>
+        <v>17.6166</v>
       </c>
       <c r="O8">
         <v>392.5668</v>
       </c>
       <c r="P8">
-        <v>15.4711221581</v>
+        <v>15.4603560565</v>
       </c>
       <c r="Q8">
         <v>0.5147550307593729</v>
@@ -5696,7 +5693,7 @@
         <v>13.71348592665002</v>
       </c>
       <c r="D9" s="4">
-        <v>0.0009364572733045003</v>
+        <v>0.0009364572733045004</v>
       </c>
       <c r="E9" s="4">
         <v>0.8876020328530302</v>
@@ -5708,13 +5705,13 @@
         <v>1.00239181729563</v>
       </c>
       <c r="H9" s="4">
-        <v>0.00312613527074461</v>
+        <v>0.003126135270744611</v>
       </c>
       <c r="I9" s="4">
-        <v>47324.15634140059</v>
+        <v>47324.1563414006</v>
       </c>
       <c r="J9" s="4">
-        <v>264.5574770388683</v>
+        <v>264.5574770388684</v>
       </c>
       <c r="K9" s="4">
         <v>-1.865161027824191</v>
@@ -5723,16 +5720,16 @@
         <v>0.8357515363213823</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q9" s="4">
         <v>-1.865161027824191</v>
@@ -5767,10 +5764,10 @@
         <v>0.004200126112959693</v>
       </c>
       <c r="I10">
-        <v>0.8511110436199741</v>
+        <v>0.8511110436199738</v>
       </c>
       <c r="J10">
-        <v>0.005999085948640937</v>
+        <v>0.005999085948640934</v>
       </c>
       <c r="K10">
         <v>2.421364011313321</v>
@@ -5782,13 +5779,13 @@
         <v>397.7362</v>
       </c>
       <c r="N10">
-        <v>18.5615</v>
+        <v>18.7193</v>
       </c>
       <c r="O10">
         <v>382.7414</v>
       </c>
       <c r="P10">
-        <v>15.6920625477</v>
+        <v>15.5550792921</v>
       </c>
       <c r="Q10">
         <v>2.421364011313321</v>
@@ -5820,7 +5817,7 @@
         <v>0.002872367027651197</v>
       </c>
       <c r="I11" s="4">
-        <v>47242.52769689465</v>
+        <v>47242.52769689466</v>
       </c>
       <c r="J11" s="4">
         <v>255.8755126776899</v>
@@ -5832,16 +5829,16 @@
         <v>1.049182169557438</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q11" s="4">
         <v>-2.527172136228328</v>
@@ -5876,7 +5873,7 @@
         <v>0.0025653847561314</v>
       </c>
       <c r="I12">
-        <v>0.02897358969802238</v>
+        <v>0.02897358969802239</v>
       </c>
       <c r="J12">
         <v>0.0001088129488181392</v>
@@ -5891,13 +5888,13 @@
         <v>420.0755</v>
       </c>
       <c r="N12">
-        <v>14.2781</v>
+        <v>14.0009</v>
       </c>
       <c r="O12">
         <v>402.4051</v>
       </c>
       <c r="P12">
-        <v>11.7405050166</v>
+        <v>11.7539290985</v>
       </c>
       <c r="Q12">
         <v>2.623220199645671</v>
@@ -5914,13 +5911,13 @@
         <v>13.71439719886068</v>
       </c>
       <c r="D13" s="4">
-        <v>0.0009508093226944609</v>
+        <v>0.0009508093226944613</v>
       </c>
       <c r="E13" s="4">
-        <v>0.8910975031795663</v>
+        <v>0.8910975031795665</v>
       </c>
       <c r="F13" s="4">
-        <v>0.00289923583108927</v>
+        <v>0.002899235831089271</v>
       </c>
       <c r="G13" s="4">
         <v>1.001191554165284</v>
@@ -5929,7 +5926,7 @@
         <v>0.002161840651871305</v>
       </c>
       <c r="I13" s="4">
-        <v>47085.20490078314</v>
+        <v>47085.20490078312</v>
       </c>
       <c r="J13" s="4">
         <v>183.8329587987095</v>
@@ -5941,16 +5938,16 @@
         <v>0.8901499197111418</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q13" s="4">
         <v>-2.505910882709017</v>
@@ -5967,7 +5964,7 @@
         <v>30</v>
       </c>
       <c r="C14">
-        <v>7.181574108241955</v>
+        <v>7.181574108241954</v>
       </c>
       <c r="D14">
         <v>0.001784814193384784</v>
@@ -5979,10 +5976,10 @@
         <v>0.002271480402933131</v>
       </c>
       <c r="G14">
-        <v>0.9800853014669939</v>
+        <v>0.9800853014669938</v>
       </c>
       <c r="H14">
-        <v>0.00350546123094885</v>
+        <v>0.003505461230948849</v>
       </c>
       <c r="I14">
         <v>1.279474424945175</v>
@@ -6000,13 +5997,13 @@
         <v>432.7757</v>
       </c>
       <c r="N14">
-        <v>21.4986</v>
+        <v>21.9775</v>
       </c>
       <c r="O14">
         <v>415.719</v>
       </c>
       <c r="P14">
-        <v>17.5169768967</v>
+        <v>17.8925037114</v>
       </c>
       <c r="Q14">
         <v>1.712729973920579</v>
@@ -6020,10 +6017,10 @@
         <v>9186</v>
       </c>
       <c r="C15" s="4">
-        <v>13.71319985415296</v>
+        <v>13.71319985415297</v>
       </c>
       <c r="D15" s="4">
-        <v>0.001149709602279575</v>
+        <v>0.001149709602279576</v>
       </c>
       <c r="E15" s="4">
         <v>0.8939406259858222</v>
@@ -6032,13 +6029,13 @@
         <v>0.003778407080398669</v>
       </c>
       <c r="G15" s="4">
-        <v>0.9988888808814648</v>
+        <v>0.9988888808814645</v>
       </c>
       <c r="H15" s="4">
         <v>0.002362222359513692</v>
       </c>
       <c r="I15" s="4">
-        <v>46823.41662719673</v>
+        <v>46823.41662719674</v>
       </c>
       <c r="J15" s="4">
         <v>226.7451110517479</v>
@@ -6050,16 +6047,16 @@
         <v>0.7914499647809169</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q15" s="4">
         <v>-2.202891300742693</v>
@@ -6082,10 +6079,10 @@
         <v>0.002357885721827777</v>
       </c>
       <c r="E16">
-        <v>17.38770470481672</v>
+        <v>17.38770470481673</v>
       </c>
       <c r="F16">
-        <v>0.03836494628929124</v>
+        <v>0.03836494628929125</v>
       </c>
       <c r="G16">
         <v>0.9845915147220022</v>
@@ -6094,7 +6091,7 @@
         <v>0.00232251073246219</v>
       </c>
       <c r="I16">
-        <v>0.04198418048932442</v>
+        <v>0.04198418048932441</v>
       </c>
       <c r="J16">
         <v>0.0001353286718302719</v>
@@ -6109,13 +6106,13 @@
         <v>454.7034</v>
       </c>
       <c r="N16">
-        <v>17.4221</v>
+        <v>17.8032</v>
       </c>
       <c r="O16">
         <v>432.406</v>
       </c>
       <c r="P16">
-        <v>13.6931576438</v>
+        <v>13.9484281894</v>
       </c>
       <c r="Q16">
         <v>2.698465868033573</v>
@@ -6132,7 +6129,7 @@
         <v>13.71319273712027</v>
       </c>
       <c r="D17" s="4">
-        <v>0.0008672834130371031</v>
+        <v>0.0008672834130371032</v>
       </c>
       <c r="E17" s="4">
         <v>0.8894925105453537</v>
@@ -6141,10 +6138,10 @@
         <v>0.003987782653041559</v>
       </c>
       <c r="G17" s="4">
-        <v>1.000439140504433</v>
+        <v>1.000439140504432</v>
       </c>
       <c r="H17" s="4">
-        <v>0.0033917317875997</v>
+        <v>0.003391731787599699</v>
       </c>
       <c r="I17" s="4">
         <v>47130.57621401784</v>
@@ -6159,16 +6156,16 @@
         <v>1.018388305285391</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q17" s="4">
         <v>-3.463886524832205</v>

</xml_diff>

<commit_message>
small QOL improvements added 'Constants' sheet
</commit_message>
<xml_diff>
--- a/data/Inga_2018-11-09_WM_20181109-114911/Results.xlsx
+++ b/data/Inga_2018-11-09_WM_20181109-114911/Results.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Calc" sheetId="2" r:id="rId2"/>
     <sheet name="Results" sheetId="3" r:id="rId3"/>
+    <sheet name="Constants" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="165">
   <si>
     <t>Lab. #</t>
   </si>
@@ -490,6 +491,120 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>R34_33</t>
+  </si>
+  <si>
+    <t>R35_33</t>
+  </si>
+  <si>
+    <t>R30_29</t>
+  </si>
+  <si>
+    <t>mf48</t>
+  </si>
+  <si>
+    <t>mf36</t>
+  </si>
+  <si>
+    <t>mf56</t>
+  </si>
+  <si>
+    <t>mf68</t>
+  </si>
+  <si>
+    <t>mf92</t>
+  </si>
+  <si>
+    <t>mf38</t>
+  </si>
+  <si>
+    <t>mf35</t>
+  </si>
+  <si>
+    <t>mf43</t>
+  </si>
+  <si>
+    <t>mf45</t>
+  </si>
+  <si>
+    <t>mf09</t>
+  </si>
+  <si>
+    <t>mf29</t>
+  </si>
+  <si>
+    <t>mf34</t>
+  </si>
+  <si>
+    <t>mf58</t>
+  </si>
+  <si>
+    <t>mf02</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>NR85</t>
+  </si>
+  <si>
+    <t>cps</t>
+  </si>
+  <si>
+    <t>slope229Correction</t>
+  </si>
+  <si>
+    <t>lambda232</t>
+  </si>
+  <si>
+    <t>lambda234</t>
+  </si>
+  <si>
+    <t>lambda238</t>
+  </si>
+  <si>
+    <t>lambda230</t>
+  </si>
+  <si>
+    <t>trisp236</t>
+  </si>
+  <si>
+    <t>trisp233</t>
+  </si>
+  <si>
+    <t>trisp229</t>
+  </si>
+  <si>
+    <t>blank234</t>
+  </si>
+  <si>
+    <t>blank234S</t>
+  </si>
+  <si>
+    <t>blank238</t>
+  </si>
+  <si>
+    <t>blank238S</t>
+  </si>
+  <si>
+    <t>blank232</t>
+  </si>
+  <si>
+    <t>blank232S</t>
+  </si>
+  <si>
+    <t>chBlank230</t>
+  </si>
+  <si>
+    <t>chBlank230S</t>
+  </si>
+  <si>
+    <t>a230232_init</t>
+  </si>
+  <si>
+    <t>a230232_init_err</t>
+  </si>
 </sst>
 </file>
 
@@ -512,7 +627,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,8 +640,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDB310"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCDCDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -543,11 +670,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -556,6 +711,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2794,11 +2955,11 @@
       <c r="AO4">
         <v>377.9962</v>
       </c>
-      <c r="AP4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>109</v>
+      <c r="AP4">
+        <v>30.0101</v>
+      </c>
+      <c r="AQ4">
+        <v>7.939259706843614</v>
       </c>
       <c r="AR4">
         <v>1.076828062108333E-07</v>
@@ -2816,13 +2977,13 @@
         <v>377.9962</v>
       </c>
       <c r="AW4">
-        <v>29.6112849037</v>
+        <v>31.4543342655</v>
       </c>
       <c r="AX4">
         <v>26.87803666683755</v>
       </c>
       <c r="AY4">
-        <v>7.833752006951393</v>
+        <v>8.321336104833858</v>
       </c>
       <c r="AZ4" t="s">
         <v>26</v>
@@ -2831,7 +2992,7 @@
         <v>11.12201138325179</v>
       </c>
       <c r="BC4">
-        <v>4.368299116375624</v>
+        <v>4.380971579467825</v>
       </c>
       <c r="BD4">
         <v>377938.2</v>
@@ -3487,10 +3648,10 @@
         <v>391.899</v>
       </c>
       <c r="AP8">
-        <v>15.5788</v>
+        <v>15.9049</v>
       </c>
       <c r="AQ8">
-        <v>3.975207897953299</v>
+        <v>4.058418112830092</v>
       </c>
       <c r="AR8">
         <v>-2.860668868070028E-06</v>
@@ -3508,13 +3669,13 @@
         <v>391.8992</v>
       </c>
       <c r="AW8">
-        <v>15.5026190881</v>
+        <v>15.5893796277</v>
       </c>
       <c r="AX8">
         <v>15.18795753431959</v>
       </c>
       <c r="AY8">
-        <v>3.955766964591915</v>
+        <v>3.977905448059092</v>
       </c>
       <c r="AZ8" t="s">
         <v>28</v>
@@ -3523,7 +3684,7 @@
         <v>1.555658449874069</v>
       </c>
       <c r="BC8">
-        <v>2.241880595005544</v>
+        <v>2.241892190473486</v>
       </c>
       <c r="BD8">
         <v>391841.2</v>
@@ -3833,10 +3994,10 @@
         <v>382.1054</v>
       </c>
       <c r="AP10">
-        <v>15.6964</v>
+        <v>15.8984</v>
       </c>
       <c r="AQ10">
-        <v>4.107871807098251</v>
+        <v>4.160736801939989</v>
       </c>
       <c r="AR10">
         <v>2.412244755611617E-05</v>
@@ -3854,13 +4015,13 @@
         <v>382.1034</v>
       </c>
       <c r="AW10">
-        <v>15.4488074363</v>
+        <v>15.7401368772</v>
       </c>
       <c r="AX10">
         <v>15.40939381408343</v>
       </c>
       <c r="AY10">
-        <v>4.043096040574357</v>
+        <v>4.119339654449554</v>
       </c>
       <c r="AZ10" t="s">
         <v>29</v>
@@ -3869,7 +4030,7 @@
         <v>7.118163405083836</v>
       </c>
       <c r="BC10">
-        <v>1.865479337799864</v>
+        <v>1.866461806351067</v>
       </c>
       <c r="BD10">
         <v>382045.4</v>
@@ -4179,10 +4340,10 @@
         <v>401.7789</v>
       </c>
       <c r="AP12">
-        <v>11.9044</v>
+        <v>12.0357</v>
       </c>
       <c r="AQ12">
-        <v>2.962923140065344</v>
+        <v>2.99560280542358</v>
       </c>
       <c r="AR12">
         <v>0.0007142489577433893</v>
@@ -4200,13 +4361,13 @@
         <v>401.721</v>
       </c>
       <c r="AW12">
-        <v>11.8853853779</v>
+        <v>11.5139317475</v>
       </c>
       <c r="AX12">
         <v>11.60461605344168</v>
       </c>
       <c r="AY12">
-        <v>2.958616895283045</v>
+        <v>2.866151320817184</v>
       </c>
       <c r="AZ12" t="s">
         <v>30</v>
@@ -4215,7 +4376,7 @@
         <v>8.150533719485544</v>
       </c>
       <c r="BC12">
-        <v>1.938156956012374</v>
+        <v>1.936970295734012</v>
       </c>
       <c r="BD12">
         <v>401663</v>
@@ -4525,10 +4686,10 @@
         <v>415.0041</v>
       </c>
       <c r="AP14">
-        <v>18.4401</v>
+        <v>18.3862</v>
       </c>
       <c r="AQ14">
-        <v>4.443353692168342</v>
+        <v>4.43036586867455</v>
       </c>
       <c r="AR14">
         <v>1.624463093515693E-05</v>
@@ -4546,13 +4707,13 @@
         <v>415.0028</v>
       </c>
       <c r="AW14">
-        <v>18.1093046309</v>
+        <v>18.2554661074</v>
       </c>
       <c r="AX14">
         <v>17.66418967999461</v>
       </c>
       <c r="AY14">
-        <v>4.363658421316676</v>
+        <v>4.398877816583407</v>
       </c>
       <c r="AZ14" t="s">
         <v>31</v>
@@ -4561,7 +4722,7 @@
         <v>5.524823909136777</v>
       </c>
       <c r="BC14">
-        <v>2.219109802415591</v>
+        <v>2.219400904872311</v>
       </c>
       <c r="BD14">
         <v>414944.8</v>
@@ -4871,10 +5032,10 @@
         <v>431.6856</v>
       </c>
       <c r="AP16">
-        <v>13.922</v>
+        <v>13.9222</v>
       </c>
       <c r="AQ16">
-        <v>3.225032292019933</v>
+        <v>3.225078622034184</v>
       </c>
       <c r="AR16">
         <v>0.0004976277241418383</v>
@@ -4892,13 +5053,13 @@
         <v>431.6452</v>
       </c>
       <c r="AW16">
-        <v>14.2254519071</v>
+        <v>14.3116825688</v>
       </c>
       <c r="AX16">
         <v>13.74048435635092</v>
       </c>
       <c r="AY16">
-        <v>3.295635375326774</v>
+        <v>3.315612583853591</v>
       </c>
       <c r="AZ16" t="s">
         <v>32</v>
@@ -4907,7 +5068,7 @@
         <v>9.123121977598503</v>
       </c>
       <c r="BC16">
-        <v>1.800615397212429</v>
+        <v>1.801068280153209</v>
       </c>
       <c r="BD16">
         <v>431587.2</v>
@@ -5334,20 +5495,20 @@
       <c r="M4">
         <v>377.9962</v>
       </c>
-      <c r="N4" t="s">
-        <v>109</v>
+      <c r="N4">
+        <v>30.0101</v>
       </c>
       <c r="O4">
         <v>377.9962</v>
       </c>
       <c r="P4">
-        <v>29.6112849037</v>
+        <v>31.4543342655</v>
       </c>
       <c r="Q4">
         <v>11.12201138325179</v>
       </c>
       <c r="R4">
-        <v>4.368299116375624</v>
+        <v>4.380971579467825</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="3" customFormat="1">
@@ -5559,19 +5720,19 @@
         <v>391.899</v>
       </c>
       <c r="N8">
-        <v>15.5788</v>
+        <v>15.9049</v>
       </c>
       <c r="O8">
         <v>391.8992</v>
       </c>
       <c r="P8">
-        <v>15.5026190881</v>
+        <v>15.5893796277</v>
       </c>
       <c r="Q8">
         <v>1.555658449874069</v>
       </c>
       <c r="R8">
-        <v>2.241880595005544</v>
+        <v>2.241892190473486</v>
       </c>
     </row>
     <row r="9" spans="1:19" s="3" customFormat="1">
@@ -5671,19 +5832,19 @@
         <v>382.1054</v>
       </c>
       <c r="N10">
-        <v>15.6964</v>
+        <v>15.8984</v>
       </c>
       <c r="O10">
         <v>382.1034</v>
       </c>
       <c r="P10">
-        <v>15.4488074363</v>
+        <v>15.7401368772</v>
       </c>
       <c r="Q10">
         <v>7.118163405083836</v>
       </c>
       <c r="R10">
-        <v>1.865479337799864</v>
+        <v>1.866461806351067</v>
       </c>
     </row>
     <row r="11" spans="1:19" s="3" customFormat="1">
@@ -5783,19 +5944,19 @@
         <v>401.7789</v>
       </c>
       <c r="N12">
-        <v>11.9044</v>
+        <v>12.0357</v>
       </c>
       <c r="O12">
         <v>401.721</v>
       </c>
       <c r="P12">
-        <v>11.8853853779</v>
+        <v>11.5139317475</v>
       </c>
       <c r="Q12">
         <v>8.150533719485544</v>
       </c>
       <c r="R12">
-        <v>1.938156956012374</v>
+        <v>1.936970295734012</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="3" customFormat="1">
@@ -5895,19 +6056,19 @@
         <v>415.0041</v>
       </c>
       <c r="N14">
-        <v>18.4401</v>
+        <v>18.3862</v>
       </c>
       <c r="O14">
         <v>415.0028</v>
       </c>
       <c r="P14">
-        <v>18.1093046309</v>
+        <v>18.2554661074</v>
       </c>
       <c r="Q14">
         <v>5.524823909136777</v>
       </c>
       <c r="R14">
-        <v>2.219109802415591</v>
+        <v>2.219400904872311</v>
       </c>
     </row>
     <row r="15" spans="1:19" s="3" customFormat="1">
@@ -6007,19 +6168,19 @@
         <v>431.6856</v>
       </c>
       <c r="N16">
-        <v>13.922</v>
+        <v>13.9222</v>
       </c>
       <c r="O16">
         <v>431.6452</v>
       </c>
       <c r="P16">
-        <v>14.2254519071</v>
+        <v>14.3116825688</v>
       </c>
       <c r="Q16">
         <v>9.123121977598503</v>
       </c>
       <c r="R16">
-        <v>1.800615397212429</v>
+        <v>1.801068280153209</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="3" customFormat="1">
@@ -6076,6 +6237,327 @@
       </c>
       <c r="R17" s="3" t="s">
         <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="5">
+        <v>0.002324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.005066</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="5">
+        <v>4.8E-05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1.336402435064349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1.008202776684838</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.334493224630051</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.665506775369946</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1.025840620457897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.673784240557133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.673784240557127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="5">
+        <v>-0.337307116990441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.336402435064353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="5">
+        <v>-0.34318587041139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="5">
+        <v>-1.025840620457897</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0.337307116990439</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.682654750046506</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="5">
+        <v>6.02214129E+23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="5">
+        <v>137.881</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="5">
+        <v>62500000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="5">
+        <v>3.4053</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="5">
+        <v>4.94752E-11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="5">
+        <v>2.82206E-06</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1.55125E-10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" s="5">
+        <v>9.1705E-06</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="5">
+        <v>3.86778</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0.038556</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" s="5">
+        <v>0.018067</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" s="5">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" s="5">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" s="5">
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>